<commit_message>
Metrics and code packaging in functions
</commit_message>
<xml_diff>
--- a/_scenarios/bateria individual sintetizado/bbce2_Factures_ficticies.xlsx
+++ b/_scenarios/bateria individual sintetizado/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>